<commit_message>
Verified all tests running as of 7/13/2018 AutoExportWeeklyAndDaySelection is broken ExportAuditLogCSV needs to add a case before it can execute GiveEditPermissionForCaseAndVerifyViewIsAlsoApplied also needs a case before it can execute ServerActivateCountry might not be valid anymore
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19413"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CDA71A5-5C9E-4734-9CB7-394D55EBD229}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imran\Katalon Studio\CommandCenterEnterprise\Data Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="17670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -13,12 +17,12 @@
     <sheet name="AddNewUser" sheetId="3" r:id="rId3"/>
     <sheet name="PermissionUser" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>OfficerID</t>
   </si>
@@ -38,9 +42,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://cbsccube8:803/#/locationselect</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -67,12 +68,21 @@
   <si>
     <t>qaiser</t>
   </si>
+  <si>
+    <t>http://cbsqar2:803/#/locationselect</t>
+  </si>
+  <si>
+    <t>SubServer</t>
+  </si>
+  <si>
+    <t>CBSQAR5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,16 +437,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4777</v>
       </c>
@@ -470,69 +480,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B880D4-CD42-4BBD-AFE9-3C451F534BA9}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{ED0E97F7-ACE7-5C6E-99EE-D5B290455111}">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="/locationselect" xr:uid="{C3A07FFF-B885-4F19-A71E-3EAEB5521502}"/>
+    <hyperlink ref="A2" r:id="rId1" location="/locationselect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B4B549-A41E-4C9A-A19A-B1F7DFF2CB7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{FA91EAAA-098D-54F2-861E-DFDC8F6E21BC}">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
       <c r="D2">
         <v>9876</v>
@@ -547,21 +567,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F67ECEF-906E-4D4F-AAA9-A1C874427803}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{4275F273-3A8D-5C16-BEAA-0AD86B10E5A9}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Refactored objects - Added add patrol unit, create case test cases - Smoke test suite creation
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -9,20 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="17670" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="17670" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="WebURL" sheetId="2" r:id="rId2"/>
     <sheet name="AddNewUser" sheetId="3" r:id="rId3"/>
-    <sheet name="PermissionUser" sheetId="4" r:id="rId4"/>
+    <sheet name="AddNewCase" sheetId="5" r:id="rId4"/>
+    <sheet name="AddNewH1Template" sheetId="6" r:id="rId5"/>
+    <sheet name="AddH1PatrolUnit" sheetId="7" r:id="rId6"/>
+    <sheet name="PermissionUser" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>OfficerID</t>
   </si>
@@ -76,6 +79,30 @@
   </si>
   <si>
     <t>CBSQAR5</t>
+  </si>
+  <si>
+    <t>AssignedTo</t>
+  </si>
+  <si>
+    <t>CaseName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TemplateName</t>
+  </si>
+  <si>
+    <t>PatrolUnitName</t>
+  </si>
+  <si>
+    <t>testcase108</t>
+  </si>
+  <si>
+    <t>test017</t>
+  </si>
+  <si>
+    <t>test018</t>
   </si>
 </sst>
 </file>
@@ -483,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -522,7 +549,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>9876</v>
+        <v>1289</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -568,9 +595,112 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4777</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>